<commit_message>
Aggiornata slide con Tabella Dati a 2 variabili
</commit_message>
<xml_diff>
--- a/exercises/documento28/AnalisiDati_1.xlsx
+++ b/exercises/documento28/AnalisiDati_1.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\excel\exercises\documento28\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91E90CD-8F28-4E89-958F-F7B18129A7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419FEF10-4A3A-49B7-93A6-FF8AA544C988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="1005" windowWidth="18915" windowHeight="12060" activeTab="1" xr2:uid="{AE25153E-9FA4-414D-BE8A-A86E5A9F2C6C}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{AE25153E-9FA4-414D-BE8A-A86E5A9F2C6C}"/>
   </bookViews>
   <sheets>
     <sheet name="TABELLA DATI ANALISI MUTUO" sheetId="1" r:id="rId1"/>
@@ -37,8 +37,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Analisi mutuo</t>
   </si>
@@ -370,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -402,6 +424,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -772,6 +797,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4826E0-E2F6-4D04-BDE5-D4250F82153F}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -871,161 +897,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85A8CD9-8819-4836-AA19-82E0B48EAF17}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="7">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="C6" s="9">
-        <v>10</v>
-      </c>
-      <c r="D6" s="9">
-        <v>15</v>
-      </c>
-      <c r="E6" s="9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="5">
-        <f>B3*B4</f>
-        <v>1750</v>
-      </c>
-      <c r="C7" s="6">
-        <f t="dataTable" ref="C7:E7" dt2D="0" dtr="1" r1="B4"/>
-        <v>3500</v>
-      </c>
-      <c r="D7" s="6">
-        <v>5250</v>
-      </c>
-      <c r="E7" s="6">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="C10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="C11" s="9">
-        <v>20</v>
-      </c>
-      <c r="D11" s="9">
-        <v>30</v>
-      </c>
-      <c r="E11" s="9">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B12" s="22">
-        <f>B3*B4</f>
-        <v>1750</v>
-      </c>
-      <c r="C12" s="6">
-        <f t="dataTable" ref="C12:E12" dt2D="0" dtr="1" r1="B4" ca="1"/>
-        <v>7000</v>
-      </c>
-      <c r="D12" s="6">
-        <v>10500</v>
-      </c>
-      <c r="E12" s="6">
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="25"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
-    </row>
-    <row r="19" spans="1:2" ht="164.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="25"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A15:B19"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A74805C-62DA-42E9-AF87-09E58497F068}">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1060,6 +935,163 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="C6" s="9">
+        <v>10</v>
+      </c>
+      <c r="D6" s="9">
+        <v>15</v>
+      </c>
+      <c r="E6" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5">
+        <f>B3*B4</f>
+        <v>1750</v>
+      </c>
+      <c r="C7" s="6">
+        <f t="dataTable" ref="C7:E7" dt2D="0" dtr="1" r1="B4"/>
+        <v>3500</v>
+      </c>
+      <c r="D7" s="6">
+        <v>5250</v>
+      </c>
+      <c r="E7" s="6">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="C10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="C11" s="9">
+        <v>20</v>
+      </c>
+      <c r="D11" s="9">
+        <v>30</v>
+      </c>
+      <c r="E11" s="9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B12" s="22">
+        <f>B3*B4</f>
+        <v>1750</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="dataTable" ref="C12:E12" dt2D="0" dtr="1" r1="B4" ca="1"/>
+        <v>7000</v>
+      </c>
+      <c r="D12" s="6">
+        <v>10500</v>
+      </c>
+      <c r="E12" s="6">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="25"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+    </row>
+    <row r="19" spans="1:2" ht="164.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A15:B19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A74805C-62DA-42E9-AF87-09E58497F068}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7">
+        <v>350</v>
+      </c>
+      <c r="D3" t="e" cm="1">
+        <f t="array" ref="D3">_xlfn.TEXTSPLIT(C3," ")</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -1068,8 +1100,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="C6" s="4" t="s">
-        <v>10</v>
+      <c r="C6" s="4" t="str">
+        <f>_xlfn.CONCAT(A6," ",B6)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D6" s="4" t="s">
         <v>11</v>
@@ -1101,7 +1134,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="6">
-        <f t="dataTable" ref="C8:E10" dt2D="1" dtr="1" r1="B4" r2="B5"/>
+        <f t="dataTable" ref="C8:E10" dt2D="1" dtr="1" r1="B4" r2="B5" ca="1"/>
         <v>3500</v>
       </c>
       <c r="D8" s="6">
@@ -1137,6 +1170,75 @@
       </c>
       <c r="E10" s="6">
         <v>21000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <f>B3*B4*B5</f>
+        <v>3500</v>
+      </c>
+      <c r="C13" s="3">
+        <v>5</v>
+      </c>
+      <c r="D13" s="3">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="26">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <f t="dataTable" ref="C14:E16" dt2D="1" dtr="1" r1="B4" r2="B5"/>
+        <v>1750</v>
+      </c>
+      <c r="D14">
+        <v>3500</v>
+      </c>
+      <c r="E14">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="26">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>3500</v>
+      </c>
+      <c r="D15">
+        <v>7000</v>
+      </c>
+      <c r="E15">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="26">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>5250</v>
+      </c>
+      <c r="D16">
+        <v>10500</v>
+      </c>
+      <c r="E16">
+        <v>15750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>